<commit_message>
some modify according to real data
</commit_message>
<xml_diff>
--- a/指標報告書自動化範例檔案/B 參數.xlsx
+++ b/指標報告書自動化範例檔案/B 參數.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\學評組工讀生\應數碩三_陳慎逸\程式學習\Index-Evaluation-Analysis-Report\指標報告書自動化範例檔案\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C7CF04-6DEC-4763-B012-A4508C5A18C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A533855-7116-4D3C-88E5-8378907F93A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="原始資料參數" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="369">
   <si>
     <t>編號</t>
   </si>
@@ -1111,10 +1111,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>國立政治大學</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>全校</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1172,35 +1168,11 @@
     <t>指標數據筆數</t>
   </si>
   <si>
-    <t>學年度</t>
-  </si>
-  <si>
-    <t>原始資料前綴</t>
-  </si>
-  <si>
-    <t>output-</t>
-  </si>
-  <si>
-    <t>原始資料後綴</t>
-  </si>
-  <si>
-    <t>_data</t>
-  </si>
-  <si>
-    <t>原始資料副檔名</t>
-  </si>
-  <si>
-    <t>.xls</t>
-  </si>
-  <si>
-    <t>資料頁名稱</t>
-  </si>
-  <si>
-    <t>標題列列號</t>
+    <t>本次指標學年度</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>近三年比較</t>
+    <t>政治大學</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2148,10 +2120,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9EF79C-B6DC-4966-8323-52D8F19EFDAE}">
-  <dimension ref="A1:B8"/>
+  <sheetPr codeName="工作表1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2162,7 +2135,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="44" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B1" s="39">
         <v>78</v>
@@ -2170,55 +2143,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B2" s="39">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="44" t="s">
-        <v>369</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>370</v>
-      </c>
-    </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="44" t="s">
-        <v>371</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="44" t="s">
-        <v>373</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="44" t="s">
-        <v>375</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="44" t="s">
-        <v>376</v>
-      </c>
-      <c r="B7" s="39">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2228,10 +2161,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="工作表2"/>
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3603,6 +3537,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8811FA-91F4-4835-A61F-1BCF00FEBC7D}">
+  <sheetPr codeName="工作表3"/>
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3618,13 +3553,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="42" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B1" s="43" t="s">
         <v>173</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3728,7 +3663,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="41" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B11" s="41" t="s">
         <v>341</v>
@@ -3739,7 +3674,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="41" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B12" s="41" t="s">
         <v>346</v>
@@ -3751,7 +3686,7 @@
     <row r="13" spans="1:3">
       <c r="A13" s="41"/>
       <c r="B13" s="41" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C13" s="41">
         <v>83</v>
@@ -3765,10 +3700,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6F4F1D-4402-498D-B742-AC62FD83CA7B}">
+  <sheetPr codeName="工作表4"/>
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75"/>
@@ -3795,16 +3731,16 @@
     </row>
     <row r="2" spans="1:4" ht="16.5">
       <c r="A2" s="30" t="s">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>351</v>
       </c>
       <c r="C2" s="30" t="s">
+        <v>368</v>
+      </c>
+      <c r="D2" s="31" t="s">
         <v>352</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5">
@@ -3815,10 +3751,10 @@
         <v>100</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5">
@@ -4056,7 +3992,7 @@
         <v>208</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.5">
@@ -4285,16 +4221,16 @@
     </row>
     <row r="37" spans="1:4" ht="16.5">
       <c r="A37" s="35" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B37" s="36">
         <v>600</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5">
@@ -4532,7 +4468,7 @@
         <v>273</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="16.5">
@@ -4840,7 +4776,7 @@
         <v>314</v>
       </c>
       <c r="D76" s="38" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="16.5">
@@ -4963,7 +4899,7 @@
         <v>900</v>
       </c>
       <c r="C85" s="25" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D85" s="26" t="s">
         <v>331</v>
@@ -5044,13 +4980,13 @@
         <v>341</v>
       </c>
       <c r="B91" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C91" s="25" t="s">
         <v>341</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="16.5">
@@ -5086,7 +5022,7 @@
         <v>346</v>
       </c>
       <c r="B94" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C94" s="25" t="s">
         <v>346</v>

</xml_diff>